<commit_message>
Refactored file names and added updated author functionality
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
   <si>
     <t>seamless-immutable</t>
   </si>
@@ -259,9 +259,6 @@
   </si>
   <si>
     <t>Fixed issue of reset value after adding author</t>
-  </si>
-  <si>
-    <t>Rahul</t>
   </si>
   <si>
     <t>Add Validation on Save button</t>
@@ -658,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -828,20 +825,20 @@
       <c r="C24" t="s">
         <v>77</v>
       </c>
-      <c r="D24" t="s">
-        <v>78</v>
+      <c r="D24" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
+      <c r="D25" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored code and added date picker
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17870"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Reactjs\ReactLearn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Dev\ReactLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
   <si>
     <t>seamless-immutable</t>
   </si>
@@ -655,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -841,15 +841,18 @@
       <c r="C26" t="s">
         <v>74</v>
       </c>
+      <c r="D26" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
         <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added level in course
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
   <si>
     <t>seamless-immutable</t>
   </si>
@@ -171,9 +171,6 @@
     <t>12. add Delete icon</t>
   </si>
   <si>
-    <t>13. Styling</t>
-  </si>
-  <si>
     <t>13. Radium pacakge for stylying</t>
   </si>
   <si>
@@ -222,12 +219,6 @@
     <t>Unsaved changes message when user is leaving manage course page</t>
   </si>
   <si>
-    <t>Modal page</t>
-  </si>
-  <si>
-    <t>Router redirect</t>
-  </si>
-  <si>
     <t>Styling of react components</t>
   </si>
   <si>
@@ -261,7 +252,19 @@
     <t>Fixed issue of reset value after adding author</t>
   </si>
   <si>
-    <t>Add Validation on Save button</t>
+    <t>Didable Save button when page loaded with blank values</t>
+  </si>
+  <si>
+    <t>WIP</t>
+  </si>
+  <si>
+    <t>Add email to author page with validation</t>
+  </si>
+  <si>
+    <t>http://react-day-picker.js.org/examples/?overlay</t>
+  </si>
+  <si>
+    <t>Add tests for author module</t>
   </si>
 </sst>
 </file>
@@ -653,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:D40"/>
+  <dimension ref="C5:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -664,235 +667,186 @@
     <col min="3" max="3" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>75</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>58</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B11">
-        <v>6</v>
-      </c>
-      <c r="C11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B12">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <v>9</v>
-      </c>
-      <c r="C14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B17">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B18">
-        <v>12</v>
-      </c>
-      <c r="C18" t="s">
+    </row>
+    <row r="32" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="C32" s="6" t="s">
         <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B19">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <v>14</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <v>15</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B22">
-        <v>16</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C33" t="s">
-        <v>76</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C36" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="37" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C38" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C39" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C40" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added logic to sort course by default on load of page
</commit_message>
<xml_diff>
--- a/Program.xlsx
+++ b/Program.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="86">
   <si>
     <t>seamless-immutable</t>
   </si>
@@ -265,13 +265,31 @@
   </si>
   <si>
     <t>Add tests for author module</t>
+  </si>
+  <si>
+    <t>debug</t>
+  </si>
+  <si>
+    <t>es6-error</t>
+  </si>
+  <si>
+    <t>helmet</t>
+  </si>
+  <si>
+    <t>moment-timezone</t>
+  </si>
+  <si>
+    <t>bluebird</t>
+  </si>
+  <si>
+    <t>classnames</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,6 +319,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color rgb="FF660E7A"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.6"/>
+      <color rgb="FF008000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -329,7 +361,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -341,6 +373,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -658,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -857,10 +895,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:D65"/>
+  <dimension ref="C5:D70"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C5" activeCellId="1" sqref="C5:C55 C5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -982,6 +1020,9 @@
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="6"/>
+      <c r="D25" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C26" s="6"/>
@@ -1168,6 +1209,31 @@
     <row r="65" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D65" s="3" t="s">
         <v>43</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="8" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>